<commit_message>
Actualizacion de Entidades en Documento
</commit_message>
<xml_diff>
--- a/1_Analisis/Analisis_Administrador_Top_Stylist.xlsx
+++ b/1_Analisis/Analisis_Administrador_Top_Stylist.xlsx
@@ -10,13 +10,14 @@
     <sheet name="RESUMEN" sheetId="1" r:id="rId1"/>
     <sheet name="ANALISIS DE ESFUERZO" sheetId="5" r:id="rId2"/>
     <sheet name="RN Ventas y Reportes" sheetId="6" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="98">
   <si>
     <t>Analisis de Funcionalidad "Administrador Top Stylist"</t>
   </si>
@@ -27,9 +28,6 @@
     <t>Alumno</t>
   </si>
   <si>
-    <t>Colegiatura</t>
-  </si>
-  <si>
     <t>Carrera</t>
   </si>
   <si>
@@ -39,18 +37,9 @@
     <t>Pago</t>
   </si>
   <si>
-    <t>Orden de Pedido</t>
-  </si>
-  <si>
     <t>Producto</t>
   </si>
   <si>
-    <t>Factura</t>
-  </si>
-  <si>
-    <t>Nota</t>
-  </si>
-  <si>
     <t>Rol</t>
   </si>
   <si>
@@ -298,13 +287,37 @@
   </si>
   <si>
     <t>Reporte de alumnos por materia</t>
+  </si>
+  <si>
+    <t>Materia</t>
+  </si>
+  <si>
+    <t>Ciclo</t>
+  </si>
+  <si>
+    <t>Orden de compra</t>
+  </si>
+  <si>
+    <t>Personal (tipo de empleado)</t>
+  </si>
+  <si>
+    <t>Alta de Curso</t>
+  </si>
+  <si>
+    <t>Alta de Materias</t>
+  </si>
+  <si>
+    <t>Registro de Pago</t>
+  </si>
+  <si>
+    <t>Nota (La Factura es un tipo de Nota)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +329,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -405,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -444,15 +471,46 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -462,9 +520,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -767,16 +836,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L42"/>
+  <dimension ref="A2:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46.5703125" bestFit="1" customWidth="1"/>
@@ -796,660 +865,683 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
+        <v>7</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>33</v>
+      <c r="C5" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+        <v>8</v>
+      </c>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="19"/>
+        <v>3</v>
+      </c>
+      <c r="C6" s="31"/>
       <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>17</v>
-      </c>
       <c r="H6" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="19"/>
+        <v>4</v>
+      </c>
+      <c r="C7" s="31"/>
       <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="26"/>
+      <c r="H7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="I7" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>24</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C8" s="31"/>
       <c r="E8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="22"/>
+        <v>11</v>
+      </c>
+      <c r="G8" s="26"/>
       <c r="H8" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="22"/>
+        <v>91</v>
+      </c>
+      <c r="C9" s="31"/>
       <c r="E9" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="G9" s="26"/>
+      <c r="H9" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="E10" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="26"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="5" t="s">
-        <v>79</v>
+      <c r="B11" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="20" t="s">
+        <v>75</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="34"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+        <v>92</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="27"/>
+      <c r="H13" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="G14" s="21" t="s">
-        <v>24</v>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="G14" s="29" t="s">
+        <v>17</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="22"/>
+        <v>43</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="5" t="s">
-        <v>27</v>
+        <v>56</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>96</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="26"/>
+      <c r="H17" s="24"/>
       <c r="I17" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="K17" s="6"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>29</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="G18" s="26"/>
       <c r="H18" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="G19" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>34</v>
+        <v>67</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" s="26"/>
+      <c r="H19" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="19"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="7" t="s">
-        <v>35</v>
+        <v>68</v>
+      </c>
+      <c r="C20" s="31"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J20" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="K20" s="6"/>
-      <c r="L20" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G21" s="22"/>
-      <c r="H21" s="7" t="s">
-        <v>36</v>
+      <c r="B21" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="31"/>
+      <c r="G21" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G22" s="23"/>
-      <c r="H22" t="s">
-        <v>56</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14" t="s">
-        <v>46</v>
+      <c r="B22" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="31"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G23" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>37</v>
+      <c r="G23" s="37"/>
+      <c r="H23" s="21" t="s">
+        <v>32</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J23" s="6"/>
-      <c r="K23" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="L23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G24" s="19"/>
-      <c r="H24" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="L24" s="6"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G25" s="19"/>
+      <c r="G25" s="29" t="s">
+        <v>11</v>
+      </c>
       <c r="H25" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
-      </c>
-      <c r="G26" s="19"/>
+        <v>51</v>
+      </c>
+      <c r="G26" s="29"/>
       <c r="H26" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="29"/>
       <c r="H27" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="29"/>
+      <c r="H28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="29"/>
+      <c r="H29" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G30" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G31" s="36"/>
+      <c r="H31" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G32" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G28" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G29" s="23"/>
-      <c r="H29" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G30" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G31" s="19"/>
-      <c r="H31" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I31" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J31" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="19"/>
-      <c r="H32" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="I32" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
     <row r="33" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G33" s="19" t="s">
-        <v>65</v>
-      </c>
+      <c r="G33" s="29"/>
       <c r="H33" s="7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J33" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
     <row r="34" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G34" s="19"/>
+      <c r="G34" s="29"/>
       <c r="H34" s="7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J34" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
     <row r="35" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G35" s="19" t="s">
-        <v>70</v>
+      <c r="G35" s="31" t="s">
+        <v>61</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>46</v>
+        <v>62</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
-      <c r="L35" s="16" t="s">
-        <v>46</v>
-      </c>
+      <c r="L35" s="4"/>
     </row>
     <row r="36" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G36" s="19"/>
+      <c r="G36" s="31"/>
       <c r="H36" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>46</v>
+        <v>63</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="16" t="s">
-        <v>46</v>
-      </c>
+      <c r="L36" s="4"/>
     </row>
     <row r="37" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G37" s="19"/>
+      <c r="G37" s="31" t="s">
+        <v>66</v>
+      </c>
       <c r="H37" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G38" s="19"/>
+      <c r="G38" s="31"/>
       <c r="H38" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G39" s="31"/>
+      <c r="H39" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="16" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G40" t="s">
-        <v>89</v>
-      </c>
-      <c r="H40" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="H41" s="25" t="s">
-        <v>91</v>
+      <c r="G40" s="31"/>
+      <c r="H40" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="16" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="H42" s="25" t="s">
-        <v>92</v>
+      <c r="G42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H43" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H44" s="19" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="G30:G32"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="G35:G38"/>
-    <mergeCell ref="G23:G27"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="G19:G22"/>
+  <mergeCells count="24">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="G37:G40"/>
+    <mergeCell ref="G25:G29"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="G21:G24"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="G6:G13"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G16:G20"/>
     <mergeCell ref="I4:L4"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="G14:G15"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="G6:G11"/>
-    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1474,55 +1566,55 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>48</v>
+      <c r="B2" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>44</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G2" s="9"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
       <c r="F3" s="12">
         <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
-        <v>17</v>
+      <c r="B4" s="32" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D4" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="22"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="13">
         <v>6</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" s="13">
         <v>6</v>
@@ -1533,30 +1625,30 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="22"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D7" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D8" s="13">
         <v>10</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D9" s="13">
         <v>8</v>
@@ -1566,34 +1658,34 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="31"/>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="13">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="13">
-        <v>8</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="D12" s="13">
         <v>8</v>
@@ -1603,27 +1695,27 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D13" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D14" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="23"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D15" s="13">
         <v>10</v>
@@ -1631,202 +1723,202 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D16" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
-        <v>12</v>
+      <c r="B17" s="32" t="s">
+        <v>8</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="33"/>
+      <c r="C18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="33"/>
+      <c r="C19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="34"/>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="31"/>
+      <c r="C22" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
-      <c r="C18" s="7" t="s">
+      <c r="D22" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="31"/>
+      <c r="C23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
-      <c r="C19" s="7" t="s">
+      <c r="D23" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="31"/>
+      <c r="C24" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="23"/>
-      <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="D24" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="31"/>
+      <c r="C25" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="7" t="s">
+      <c r="D25" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="7" t="s">
+      <c r="D26" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="34"/>
+      <c r="C27" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="23"/>
-      <c r="C27" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="D27" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="31"/>
+      <c r="C29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="31"/>
+      <c r="C30" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="7" t="s">
+      <c r="D31" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="31"/>
+      <c r="C32" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="7" t="s">
+      <c r="D32" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="C32" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="19" t="s">
+      <c r="C33" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="D33" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D34" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D35" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
+      <c r="B36" s="31"/>
       <c r="C36" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D36" s="13">
         <v>8</v>
@@ -1834,7 +1926,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C37" s="10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D37" s="11">
         <f>SUM(D4:D36)</f>
@@ -1843,7 +1935,7 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C39" s="10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D39" s="11">
         <f>D37*F12</f>
@@ -1852,7 +1944,7 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C40" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D40" s="11">
         <f>D39*0.16</f>
@@ -1861,7 +1953,7 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C41" s="17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D41" s="17">
         <f>D39+D40</f>
@@ -1903,39 +1995,53 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se cambio el menu lateral por menubar
</commit_message>
<xml_diff>
--- a/1_Analisis/Analisis_Administrador_Top_Stylist.xlsx
+++ b/1_Analisis/Analisis_Administrador_Top_Stylist.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VOSTRO\Documents\GitHub\ts\1_Analisis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="23715" windowHeight="9975"/>
   </bookViews>
@@ -12,7 +17,7 @@
     <sheet name="RN Ventas y Reportes" sheetId="6" r:id="rId3"/>
     <sheet name="Hoja1" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -360,7 +365,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,6 +381,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -496,18 +507,45 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -517,47 +555,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -568,6 +574,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -616,7 +625,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -651,7 +660,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -863,7 +872,7 @@
   <dimension ref="A2:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E9" activeCellId="3" sqref="E6 E7 E8 E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,34 +907,34 @@
       <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="23" t="s">
         <v>98</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="27" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
       <c r="I5" s="3" t="s">
         <v>9</v>
       </c>
@@ -940,15 +949,15 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="27"/>
+      <c r="E6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="33" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="5" t="s">
@@ -964,15 +973,15 @@
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="E7" s="4" t="s">
+      <c r="C7" s="27"/>
+      <c r="E7" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="36"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="5" t="s">
         <v>14</v>
       </c>
@@ -986,15 +995,15 @@
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="E8" s="4" t="s">
+      <c r="C8" s="27"/>
+      <c r="E8" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="36"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="5" t="s">
         <v>16</v>
       </c>
@@ -1008,54 +1017,54 @@
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="E9" s="8" t="s">
+      <c r="C9" s="27"/>
+      <c r="E9" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="30" t="s">
+      <c r="G9" s="34"/>
+      <c r="H9" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
+      <c r="I9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="30" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="23" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="G11" s="36"/>
+      <c r="C11" s="31"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="20" t="s">
         <v>72</v>
       </c>
@@ -1069,10 +1078,10 @@
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="34"/>
-      <c r="G12" s="36"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="32"/>
+      <c r="G12" s="34"/>
       <c r="H12" s="20" t="s">
         <v>91</v>
       </c>
@@ -1082,16 +1091,16 @@
       <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="37"/>
+      <c r="G13" s="35"/>
       <c r="H13" s="20" t="s">
         <v>92</v>
       </c>
@@ -1101,11 +1110,11 @@
       <c r="L13" s="18"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="26"/>
+      <c r="C14" s="27"/>
       <c r="G14" s="25" t="s">
         <v>17</v>
       </c>
@@ -1122,11 +1131,11 @@
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="8" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="27"/>
       <c r="G15" s="25"/>
       <c r="H15" s="5" t="s">
         <v>19</v>
@@ -1141,17 +1150,17 @@
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="8" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="39" t="s">
         <v>56</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="G16" s="35" t="s">
+      <c r="G16" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="28" t="s">
         <v>93</v>
       </c>
       <c r="I16" s="6" t="s">
@@ -1164,17 +1173,17 @@
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="31"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="29"/>
       <c r="I17" s="6" t="s">
         <v>42</v>
       </c>
@@ -1185,12 +1194,12 @@
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="8" t="s">
+      <c r="A18" s="23"/>
+      <c r="B18" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="G18" s="36"/>
+      <c r="C18" s="27"/>
+      <c r="G18" s="34"/>
       <c r="H18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1204,16 +1213,16 @@
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="23" t="s">
         <v>101</v>
       </c>
       <c r="B19" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="G19" s="36"/>
+      <c r="G19" s="34"/>
       <c r="H19" s="5" t="s">
         <v>41</v>
       </c>
@@ -1229,10 +1238,10 @@
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="26"/>
-      <c r="G20" s="37"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="27"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="5" t="s">
         <v>24</v>
       </c>
@@ -1246,10 +1255,10 @@
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="26"/>
-      <c r="G21" s="27" t="s">
+      <c r="A21" s="23"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="27"/>
+      <c r="G21" s="36" t="s">
         <v>8</v>
       </c>
       <c r="H21" s="21" t="s">
@@ -1265,10 +1274,10 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="26"/>
-      <c r="G22" s="29"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="27"/>
+      <c r="G22" s="38"/>
       <c r="H22" s="21" t="s">
         <v>31</v>
       </c>
@@ -1282,16 +1291,16 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="G23" s="29"/>
+      <c r="G23" s="38"/>
       <c r="H23" s="21" t="s">
         <v>32</v>
       </c>
@@ -1305,12 +1314,12 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="8" t="s">
+      <c r="A24" s="23"/>
+      <c r="B24" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="G24" s="28"/>
+      <c r="C24" s="23"/>
+      <c r="G24" s="37"/>
       <c r="H24" s="22" t="s">
         <v>52</v>
       </c>
@@ -1396,7 +1405,7 @@
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G30" s="27" t="s">
+      <c r="G30" s="36" t="s">
         <v>38</v>
       </c>
       <c r="H30" s="7" t="s">
@@ -1412,7 +1421,7 @@
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G31" s="28"/>
+      <c r="G31" s="37"/>
       <c r="H31" s="7" t="s">
         <v>40</v>
       </c>
@@ -1479,7 +1488,7 @@
       <c r="B35" t="s">
         <v>54</v>
       </c>
-      <c r="G35" s="26" t="s">
+      <c r="G35" s="27" t="s">
         <v>61</v>
       </c>
       <c r="H35" s="7" t="s">
@@ -1493,7 +1502,7 @@
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G36" s="26"/>
+      <c r="G36" s="27"/>
       <c r="H36" s="7" t="s">
         <v>63</v>
       </c>
@@ -1505,7 +1514,7 @@
       <c r="L36" s="4"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G37" s="26" t="s">
+      <c r="G37" s="27" t="s">
         <v>66</v>
       </c>
       <c r="H37" s="7" t="s">
@@ -1521,7 +1530,7 @@
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G38" s="26"/>
+      <c r="G38" s="27"/>
       <c r="H38" s="7" t="s">
         <v>68</v>
       </c>
@@ -1535,7 +1544,7 @@
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G39" s="26"/>
+      <c r="G39" s="27"/>
       <c r="H39" s="7" t="s">
         <v>69</v>
       </c>
@@ -1549,7 +1558,7 @@
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G40" s="26"/>
+      <c r="G40" s="27"/>
       <c r="H40" s="7" t="s">
         <v>70</v>
       </c>
@@ -1582,26 +1591,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="G6:G13"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G16:G20"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G32:G34"/>
     <mergeCell ref="G35:G36"/>
@@ -1614,6 +1603,26 @@
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="G6:G13"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G16:G20"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A19:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1638,13 +1647,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="26" t="s">
         <v>44</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1653,15 +1662,15 @@
       <c r="G2" s="9"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
       <c r="F3" s="12">
         <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1672,7 +1681,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="33"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
@@ -1684,7 +1693,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="33"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1697,7 +1706,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="33"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
@@ -1706,7 +1715,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="33"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="5" t="s">
         <v>71</v>
       </c>
@@ -1718,7 +1727,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="34"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="5" t="s">
         <v>72</v>
       </c>
@@ -1730,7 +1739,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="27" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1741,7 +1750,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
@@ -1753,7 +1762,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="30" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1767,7 +1776,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="33"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="5" t="s">
         <v>22</v>
       </c>
@@ -1776,7 +1785,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="33"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="5" t="s">
         <v>23</v>
       </c>
@@ -1785,7 +1794,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="5" t="s">
         <v>41</v>
       </c>
@@ -1805,7 +1814,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -1816,7 +1825,7 @@
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="33"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="7" t="s">
         <v>31</v>
       </c>
@@ -1825,7 +1834,7 @@
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="33"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="7" t="s">
         <v>32</v>
       </c>
@@ -1834,7 +1843,7 @@
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="34"/>
+      <c r="B20" s="32"/>
       <c r="C20" t="s">
         <v>52</v>
       </c>
@@ -1843,7 +1852,7 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -1854,7 +1863,7 @@
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="26"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="7" t="s">
         <v>34</v>
       </c>
@@ -1863,7 +1872,7 @@
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="26"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="7" t="s">
         <v>35</v>
       </c>
@@ -1872,7 +1881,7 @@
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="26"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="7" t="s">
         <v>36</v>
       </c>
@@ -1881,7 +1890,7 @@
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="26"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="7" t="s">
         <v>37</v>
       </c>
@@ -1890,7 +1899,7 @@
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="30" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1901,7 +1910,7 @@
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="34"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="7" t="s">
         <v>40</v>
       </c>
@@ -1910,7 +1919,7 @@
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="27" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -1921,7 +1930,7 @@
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="26"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="7" t="s">
         <v>59</v>
       </c>
@@ -1930,7 +1939,7 @@
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="26"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="7" t="s">
         <v>60</v>
       </c>
@@ -1939,7 +1948,7 @@
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="27" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -1950,7 +1959,7 @@
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="26"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="7" t="s">
         <v>63</v>
       </c>
@@ -1959,7 +1968,7 @@
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="27" t="s">
         <v>66</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -1970,7 +1979,7 @@
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="26"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="7" t="s">
         <v>68</v>
       </c>
@@ -1979,7 +1988,7 @@
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="26"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="7" t="s">
         <v>69</v>
       </c>
@@ -1988,7 +1997,7 @@
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="26"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="7" t="s">
         <v>70</v>
       </c>
@@ -2034,18 +2043,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="B26:B27"/>
     <mergeCell ref="B12:B15"/>
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="B26:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agrego el sub menu de Servicios
</commit_message>
<xml_diff>
--- a/1_Analisis/Analisis_Administrador_Top_Stylist.xlsx
+++ b/1_Analisis/Analisis_Administrador_Top_Stylist.xlsx
@@ -365,7 +365,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +387,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -488,28 +494,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -544,15 +543,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -564,6 +554,61 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" activeCellId="3" sqref="E6 E7 E8 E9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30:L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,34 +952,34 @@
       <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="20" t="s">
         <v>98</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="24" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="3" t="s">
         <v>9</v>
       </c>
@@ -949,15 +994,15 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="E6" s="39" t="s">
+      <c r="C6" s="24"/>
+      <c r="E6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="30" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="5" t="s">
@@ -973,15 +1018,15 @@
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="E7" s="39" t="s">
+      <c r="C7" s="24"/>
+      <c r="E7" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="34"/>
+      <c r="G7" s="31"/>
       <c r="H7" s="5" t="s">
         <v>14</v>
       </c>
@@ -995,15 +1040,15 @@
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="E8" s="39" t="s">
+      <c r="C8" s="24"/>
+      <c r="E8" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="34"/>
+      <c r="G8" s="31"/>
       <c r="H8" s="5" t="s">
         <v>16</v>
       </c>
@@ -1017,105 +1062,105 @@
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="E9" s="39" t="s">
+      <c r="C9" s="24"/>
+      <c r="E9" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="28" t="s">
+      <c r="G9" s="31"/>
+      <c r="H9" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
+      <c r="I9" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="40" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="20" t="s">
+      <c r="C11" s="28"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="I11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="32"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="20" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="29"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="35"/>
-      <c r="H13" s="20" t="s">
+      <c r="G13" s="32"/>
+      <c r="H13" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="39" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="G14" s="25" t="s">
+      <c r="C14" s="24"/>
+      <c r="G14" s="22" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="5" t="s">
@@ -1131,12 +1176,12 @@
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="39" t="s">
+      <c r="A15" s="20"/>
+      <c r="B15" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="G15" s="25"/>
+      <c r="C15" s="24"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="5" t="s">
         <v>19</v>
       </c>
@@ -1150,424 +1195,424 @@
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="39" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="I16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
+      <c r="I16" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="39" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="5" t="s">
+      <c r="C18" s="24"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
+      <c r="I18" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="5" t="s">
+      <c r="G19" s="53"/>
+      <c r="H19" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L19" s="6"/>
+      <c r="I19" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="L19" s="47"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="27"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="5" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="24"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
+      <c r="I20" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="27"/>
-      <c r="G21" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="21" t="s">
+      <c r="A21" s="20"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="24"/>
+      <c r="G21" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6" t="s">
+      <c r="I21" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="27"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="21" t="s">
+      <c r="A22" s="20"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="24"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6" t="s">
+      <c r="I22" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="G23" s="38"/>
-      <c r="H23" s="21" t="s">
+      <c r="G23" s="48"/>
+      <c r="H23" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6" t="s">
+      <c r="I23" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="39" t="s">
+      <c r="A24" s="20"/>
+      <c r="B24" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="22" t="s">
+      <c r="C24" s="20"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="I24" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14" t="s">
+      <c r="I24" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G25" s="25" t="s">
+      <c r="G25" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="I25" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L25" s="6"/>
+      <c r="I25" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="L25" s="37"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G26" s="25"/>
-      <c r="H26" s="7" t="s">
+      <c r="G26" s="41"/>
+      <c r="H26" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="I26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L26" s="6"/>
+      <c r="I26" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26" s="37"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G27" s="25"/>
-      <c r="H27" s="7" t="s">
+      <c r="G27" s="41"/>
+      <c r="H27" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L27" s="6"/>
+      <c r="I27" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="L27" s="37"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G28" s="25"/>
-      <c r="H28" s="7" t="s">
+      <c r="G28" s="41"/>
+      <c r="H28" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="I28" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L28" s="6"/>
+      <c r="I28" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28" s="37"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G29" s="25"/>
-      <c r="H29" s="7" t="s">
+      <c r="G29" s="41"/>
+      <c r="H29" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="I29" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L29" s="6"/>
+      <c r="I29" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="L29" s="37"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G30" s="36" t="s">
+      <c r="G30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="H30" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="I30" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
+      <c r="I30" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J30" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G31" s="37"/>
-      <c r="H31" s="7" t="s">
+      <c r="G31" s="40"/>
+      <c r="H31" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="I31" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
+      <c r="I31" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J31" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>51</v>
       </c>
-      <c r="G32" s="25" t="s">
+      <c r="G32" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="H32" s="7" t="s">
+      <c r="H32" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="I32" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="J32" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
+      <c r="I32" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G33" s="25"/>
-      <c r="H33" s="7" t="s">
+      <c r="G33" s="41"/>
+      <c r="H33" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="I33" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="J33" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
+      <c r="I33" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>53</v>
       </c>
-      <c r="G34" s="25"/>
-      <c r="H34" s="7" t="s">
+      <c r="G34" s="41"/>
+      <c r="H34" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="I34" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
+      <c r="I34" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>54</v>
       </c>
-      <c r="G35" s="27" t="s">
+      <c r="G35" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="H35" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="I35" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
+      <c r="I35" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G36" s="27"/>
-      <c r="H36" s="7" t="s">
+      <c r="G36" s="43"/>
+      <c r="H36" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="I36" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
+      <c r="I36" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G37" s="27" t="s">
+      <c r="G37" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="H37" s="7" t="s">
+      <c r="H37" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="I37" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="16" t="s">
+      <c r="I37" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="42" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G38" s="27"/>
-      <c r="H38" s="7" t="s">
+      <c r="G38" s="43"/>
+      <c r="H38" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="I38" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="16" t="s">
+      <c r="I38" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J38" s="33"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="42" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G39" s="27"/>
-      <c r="H39" s="7" t="s">
+      <c r="G39" s="43"/>
+      <c r="H39" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="I39" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="16" t="s">
+      <c r="I39" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="42" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G40" s="27"/>
-      <c r="H40" s="7" t="s">
+      <c r="G40" s="43"/>
+      <c r="H40" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="I40" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="16" t="s">
+      <c r="I40" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="42" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1575,17 +1620,17 @@
       <c r="G42" t="s">
         <v>82</v>
       </c>
-      <c r="H42" s="19" t="s">
+      <c r="H42" s="18" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H43" s="19" t="s">
+      <c r="H43" s="18" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H44" s="19" t="s">
+      <c r="H44" s="18" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1647,13 +1692,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="23" t="s">
         <v>44</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1662,15 +1707,15 @@
       <c r="G2" s="9"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
       <c r="F3" s="12">
         <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1681,7 +1726,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="31"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
@@ -1693,7 +1738,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="31"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1706,7 +1751,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
@@ -1715,7 +1760,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="31"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="5" t="s">
         <v>71</v>
       </c>
@@ -1727,7 +1772,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="5" t="s">
         <v>72</v>
       </c>
@@ -1739,7 +1784,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1750,7 +1795,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="27"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
@@ -1762,7 +1807,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="27" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1776,7 +1821,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="31"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="5" t="s">
         <v>22</v>
       </c>
@@ -1785,7 +1830,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="31"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="5" t="s">
         <v>23</v>
       </c>
@@ -1794,7 +1839,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="32"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="5" t="s">
         <v>41</v>
       </c>
@@ -1803,7 +1848,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -1814,7 +1859,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="27" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -1825,7 +1870,7 @@
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="31"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="7" t="s">
         <v>31</v>
       </c>
@@ -1834,7 +1879,7 @@
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="31"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="7" t="s">
         <v>32</v>
       </c>
@@ -1843,7 +1888,7 @@
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
+      <c r="B20" s="29"/>
       <c r="C20" t="s">
         <v>52</v>
       </c>
@@ -1852,7 +1897,7 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="24" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -1863,7 +1908,7 @@
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="27"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="7" t="s">
         <v>34</v>
       </c>
@@ -1872,7 +1917,7 @@
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="27"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="7" t="s">
         <v>35</v>
       </c>
@@ -1881,7 +1926,7 @@
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="27"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="7" t="s">
         <v>36</v>
       </c>
@@ -1890,7 +1935,7 @@
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="7" t="s">
         <v>37</v>
       </c>
@@ -1899,7 +1944,7 @@
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="27" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1910,7 +1955,7 @@
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="32"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="7" t="s">
         <v>40</v>
       </c>
@@ -1919,7 +1964,7 @@
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="24" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -1930,7 +1975,7 @@
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="27"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="7" t="s">
         <v>59</v>
       </c>
@@ -1939,7 +1984,7 @@
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="27"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="7" t="s">
         <v>60</v>
       </c>
@@ -1948,7 +1993,7 @@
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="24" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -1959,7 +2004,7 @@
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="27"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="7" t="s">
         <v>63</v>
       </c>
@@ -1968,7 +2013,7 @@
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="24" t="s">
         <v>66</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -1979,7 +2024,7 @@
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="27"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="7" t="s">
         <v>68</v>
       </c>
@@ -1988,7 +2033,7 @@
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="27"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="7" t="s">
         <v>69</v>
       </c>
@@ -1997,7 +2042,7 @@
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="27"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="7" t="s">
         <v>70</v>
       </c>
@@ -2033,10 +2078,10 @@
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="16">
         <f>D39+D40</f>
         <v>34819.487999999998</v>
       </c>

</xml_diff>